<commit_message>
updated notes to be more user friendly
</commit_message>
<xml_diff>
--- a/ModelAutoBuild/ModelAutoBuild.xlsx
+++ b/ModelAutoBuild/ModelAutoBuild.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/mikova_microsoft_com/Documents/Power BI CAT/ModelAutoBuild/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/mikova_microsoft_com/Documents/Power BI CAT/ModelAutoBuild/GitHub/v1.1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="455" documentId="8_{CFACD04C-7A0A-42D0-93DE-D5298EAD720C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{18B1B2D4-C1A0-46F8-B751-54EE1CD35AF2}"/>
+  <xr:revisionPtr revIDLastSave="477" documentId="8_{CFACD04C-7A0A-42D0-93DE-D5298EAD720C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{850CA345-F752-4651-AAB2-5A5B55FD1B84}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{BEC676D7-2196-4582-B754-27C40BA62468}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="CFB">Lists!$A$2:$A$3</definedName>
     <definedName name="DS">Lists!$C$2</definedName>
     <definedName name="DT">Lists!$F$3:$F$7</definedName>
-    <definedName name="FS">Lists!$B$2:$B$5</definedName>
+    <definedName name="FS">Lists!$B$2:$B$6</definedName>
     <definedName name="MP">Lists!$H$2:$H$3</definedName>
     <definedName name="OT">Lists!$G$2:$G$3</definedName>
     <definedName name="Prov">Lists!$E$2:$E$6</definedName>
@@ -83,6 +83,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9DEB08A6-FB34-4D17-9D85-5A3632757583}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Choose the provider (a.k.a. source type).</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -213,6 +237,92 @@
     <author>Michael Kovalsky</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AEB0147F-F0F6-4153-BB88-FBB7D59C1474}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Add the name of a measure or column. Use a friendly name (with spaces and easy to read)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{AD48ADB9-6620-4F44-99A4-E6C6F02E5CED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Add the name of the table to which the object belongs.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{28B53054-B0A5-45A3-82C3-06DD0A90DD0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Specify whether the object is a measure or a column.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B34C1912-F015-47DF-8D62-1AD56B42214A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Specify the column name from the source - must match the column in the data warehouse. For columns only.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{0C25DD3A-B438-4F71-AF8B-9DF5E1F83B10}">
       <text>
         <r>
@@ -227,6 +337,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1EF11733-8A38-4D45-81F8-8E98E5B33FEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Enter the DAX formula here - for measures only.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C8875439-6C68-4340-A6C3-8A77F5CC2B5C}">
       <text>
         <r>
@@ -266,6 +400,30 @@
             <charset val="1"/>
           </rPr>
           <t>Mark 'Yes' if the column is the primary key (must be unique in that table).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{AA9B1828-9EA6-4EC3-8AF4-AF2208079E19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Enter 'None' if the column is not summarizable.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -796,8 +954,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>409576</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -812,8 +970,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7500938" y="423863"/>
-          <a:ext cx="3433763" cy="2252663"/>
+          <a:off x="7500938" y="361950"/>
+          <a:ext cx="3433763" cy="2014538"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -875,6 +1033,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1177,7 +1339,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1284,7 +1446,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD12"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1336,7 +1498,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1347,7 +1509,7 @@
     <col min="4" max="4" width="17.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.265625" customWidth="1"/>
-    <col min="7" max="7" width="8.73046875" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.46484375" bestFit="1" customWidth="1"/>
@@ -1518,7 +1680,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1680,23 +1842,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="beaba498-6342-4421-a18c-7bfd16d38d53" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCC0D0C0DFF8C6449DE7873A14FBCB83" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fa404479abba3feb074acc2e806565cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9e548fd3-f7b4-490c-9d07-36be117e6ce5" xmlns:ns4="beaba498-6342-4421-a18c-7bfd16d38d53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25dd324ff6cedc5a2df3109d58df23e8" ns3:_="" ns4:_="">
     <xsd:import namespace="9e548fd3-f7b4-490c-9d07-36be117e6ce5"/>
@@ -1931,25 +2076,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="beaba498-6342-4421-a18c-7bfd16d38d53" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2275932-CD7C-4B19-A948-199D3E0E5FFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9805D712-353E-429A-8628-FA34CABB75D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="beaba498-6342-4421-a18c-7bfd16d38d53"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F812E1F2-546D-4113-A992-5C4A89A4B9AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1966,4 +2110,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9805D712-353E-429A-8628-FA34CABB75D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="beaba498-6342-4421-a18c-7bfd16d38d53"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2275932-CD7C-4B19-A948-199D3E0E5FFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>